<commit_message>
Sample Final Version Include 36V 薄型 設定及LED display
</commit_message>
<xml_diff>
--- a/New_LEVD1_measement.xlsx
+++ b/New_LEVD1_measement.xlsx
@@ -1260,6 +1260,60 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1271,60 +1325,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,7 +1354,7 @@
           <c:x val="7.2207084468664848E-2"/>
           <c:y val="6.5645584362161905E-2"/>
           <c:w val="0.60354223433242504"/>
-          <c:h val="0.81619343223621355"/>
+          <c:h val="0.81619343223621366"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1629,11 +1629,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="93277568"/>
-        <c:axId val="93279744"/>
+        <c:axId val="91951488"/>
+        <c:axId val="91953408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93277568"/>
+        <c:axId val="91951488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,12 +1666,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93279744"/>
+        <c:crossAx val="91953408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93279744"/>
+        <c:axId val="91953408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93277568"/>
+        <c:crossAx val="91951488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1736,7 +1736,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72070844686648583"/>
+          <c:x val="0.72070844686648594"/>
           <c:y val="0.41794355377243081"/>
           <c:w val="0.26839237057220738"/>
           <c:h val="0.11159749341567524"/>
@@ -1804,7 +1804,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,8 +1822,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10252109253634827"/>
           <c:y val="7.6923269539436984E-2"/>
-          <c:w val="0.50084074714478388"/>
-          <c:h val="0.78461734930225591"/>
+          <c:w val="0.50084074714478399"/>
+          <c:h val="0.78461734930225568"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2170,11 +2170,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="93922432"/>
-        <c:axId val="93924352"/>
+        <c:axId val="91998080"/>
+        <c:axId val="92934144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93922432"/>
+        <c:axId val="91998080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,12 +2207,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93924352"/>
+        <c:crossAx val="92934144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93924352"/>
+        <c:axId val="92934144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2255,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93922432"/>
+        <c:crossAx val="91998080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2277,9 +2277,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65210137547710112"/>
+          <c:x val="0.65210137547710123"/>
           <c:y val="0.40512921957436798"/>
-          <c:w val="0.33445405597923505"/>
+          <c:w val="0.33445405597923517"/>
           <c:h val="0.13076955821704281"/>
         </c:manualLayout>
       </c:layout>
@@ -2345,7 +2345,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2361,10 +2361,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2902387340947547E-2"/>
-          <c:y val="8.1301028172182557E-2"/>
+          <c:x val="7.2902387340947575E-2"/>
+          <c:y val="8.1301028172182571E-2"/>
           <c:w val="0.79229764355444865"/>
-          <c:h val="0.77235976763573388"/>
+          <c:h val="0.772359767635734"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2591,11 +2591,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94284800"/>
-        <c:axId val="94291072"/>
+        <c:axId val="93093888"/>
+        <c:axId val="93095808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94284800"/>
+        <c:axId val="93093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,12 +2628,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94291072"/>
+        <c:crossAx val="93095808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94291072"/>
+        <c:axId val="93095808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2676,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94284800"/>
+        <c:crossAx val="93093888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2698,10 +2698,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89408588248331877"/>
-          <c:y val="0.39837503804369434"/>
+          <c:x val="0.89408588248331888"/>
+          <c:y val="0.3983750380436944"/>
           <c:w val="9.4910655217460005E-2"/>
-          <c:h val="0.13821174789271037"/>
+          <c:h val="0.13821174789271043"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2766,7 +2766,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3166,7 +3166,7 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3175,7 +3175,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10">
-      <c r="C2" s="73">
+      <c r="C2" s="60">
         <v>41052</v>
       </c>
       <c r="E2" t="s">
@@ -3189,7 +3189,7 @@
       <c r="D4" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="61">
         <v>1.6962000000000001E-2</v>
       </c>
       <c r="F4" t="s">
@@ -3198,67 +3198,71 @@
     </row>
     <row r="5" spans="3:10" ht="17.25" thickBot="1"/>
     <row r="6" spans="3:10" ht="17.25" thickTop="1">
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79">
-        <v>48000</v>
+      <c r="D6" s="65"/>
+      <c r="E6" s="63">
+        <v>36000</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="75">
-        <v>822</v>
+      <c r="I6" s="68"/>
+      <c r="J6" s="62">
+        <v>814</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="81"/>
+      <c r="D7" s="67"/>
       <c r="E7" s="58">
         <f>ROUND(E6*E4,0)</f>
-        <v>814</v>
+        <v>611</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="76"/>
+      <c r="I7" s="68"/>
       <c r="J7">
         <f>ROUND(J6/E4,0)</f>
-        <v>48461</v>
+        <v>47990</v>
       </c>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="81"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="59">
-        <v>822</v>
+        <v>597</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="81"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="58">
         <f>E8-E7</f>
-        <v>8</v>
+        <v>-14</v>
       </c>
       <c r="F9" s="58" t="s">
         <v>145</v>
       </c>
       <c r="G9" s="15"/>
+      <c r="H9" t="str">
+        <f>DEC2HEX(E9)</f>
+        <v>FFFFFFFFF2</v>
+      </c>
     </row>
     <row r="10" spans="3:10" ht="17.25" thickBot="1">
       <c r="C10" s="45"/>
@@ -3420,18 +3424,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="10"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="60"/>
-      <c r="K5" s="64" t="s">
+      <c r="J5" s="78"/>
+      <c r="K5" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64" t="s">
+      <c r="L5" s="69"/>
+      <c r="M5" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="68"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="3:14" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -3449,20 +3453,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="79">
         <v>3000</v>
       </c>
-      <c r="J6" s="61"/>
-      <c r="K6" s="65">
+      <c r="J6" s="79"/>
+      <c r="K6" s="71">
         <f>I6*E10+E9</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65">
+      <c r="L6" s="71"/>
+      <c r="M6" s="71">
         <f>I6/10</f>
         <v>300</v>
       </c>
-      <c r="N6" s="69"/>
+      <c r="N6" s="72"/>
     </row>
     <row r="7" spans="3:14" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -3485,20 +3489,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="80">
         <v>3000</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="66">
+      <c r="J7" s="80"/>
+      <c r="K7" s="73">
         <f>I7*E13+E12</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66">
+      <c r="L7" s="73"/>
+      <c r="M7" s="73">
         <f>I7/10</f>
         <v>300</v>
       </c>
-      <c r="N7" s="70"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="3:14">
       <c r="C8" s="42" t="s">
@@ -3513,18 +3517,18 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="63" t="s">
+      <c r="I8" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="63"/>
-      <c r="K8" s="67" t="s">
+      <c r="J8" s="81"/>
+      <c r="K8" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67" t="s">
+      <c r="L8" s="75"/>
+      <c r="M8" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="71"/>
+      <c r="N8" s="76"/>
     </row>
     <row r="9" spans="3:14" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -3541,20 +3545,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="62">
+      <c r="I9" s="80">
         <v>20</v>
       </c>
-      <c r="J9" s="62"/>
-      <c r="K9" s="66">
+      <c r="J9" s="80"/>
+      <c r="K9" s="73">
         <f>I9/(E14+E15)*E15*1000/D6+E16</f>
         <v>339.23926380368101</v>
       </c>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66">
+      <c r="L9" s="73"/>
+      <c r="M9" s="73">
         <f>I9/10</f>
         <v>2</v>
       </c>
-      <c r="N9" s="72"/>
+      <c r="N9" s="77"/>
     </row>
     <row r="10" spans="3:14">
       <c r="C10" s="43" t="s">
@@ -3788,21 +3792,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2012/05/24	修改Calibration_Func()之Blink flag 2012/05/24	修改_CYCLECOUNT 參數150及500
</commit_message>
<xml_diff>
--- a/New_LEVD1_measement.xlsx
+++ b/New_LEVD1_measement.xlsx
@@ -1287,33 +1287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1324,6 +1297,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1354,7 +1354,7 @@
           <c:x val="7.2207084468664848E-2"/>
           <c:y val="6.5645584362161905E-2"/>
           <c:w val="0.60354223433242504"/>
-          <c:h val="0.81619343223621366"/>
+          <c:h val="0.81619343223621377"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1629,11 +1629,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91951488"/>
-        <c:axId val="91953408"/>
+        <c:axId val="64291200"/>
+        <c:axId val="64293120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91951488"/>
+        <c:axId val="64291200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,12 +1666,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91953408"/>
+        <c:crossAx val="64293120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91953408"/>
+        <c:axId val="64293120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91951488"/>
+        <c:crossAx val="64291200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1736,7 +1736,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72070844686648594"/>
+          <c:x val="0.72070844686648605"/>
           <c:y val="0.41794355377243081"/>
           <c:w val="0.26839237057220738"/>
           <c:h val="0.11159749341567524"/>
@@ -1804,7 +1804,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,8 +1822,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10252109253634827"/>
           <c:y val="7.6923269539436984E-2"/>
-          <c:w val="0.50084074714478399"/>
-          <c:h val="0.78461734930225568"/>
+          <c:w val="0.5008407471447841"/>
+          <c:h val="0.78461734930225546"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2170,11 +2170,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91998080"/>
-        <c:axId val="92934144"/>
+        <c:axId val="64337792"/>
+        <c:axId val="65929216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91998080"/>
+        <c:axId val="64337792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,12 +2207,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92934144"/>
+        <c:crossAx val="65929216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92934144"/>
+        <c:axId val="65929216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2255,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91998080"/>
+        <c:crossAx val="64337792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2277,9 +2277,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65210137547710123"/>
+          <c:x val="0.65210137547710134"/>
           <c:y val="0.40512921957436798"/>
-          <c:w val="0.33445405597923517"/>
+          <c:w val="0.33445405597923528"/>
           <c:h val="0.13076955821704281"/>
         </c:manualLayout>
       </c:layout>
@@ -2345,7 +2345,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2361,10 +2361,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2902387340947575E-2"/>
-          <c:y val="8.1301028172182571E-2"/>
+          <c:x val="7.2902387340947603E-2"/>
+          <c:y val="8.1301028172182599E-2"/>
           <c:w val="0.79229764355444865"/>
-          <c:h val="0.772359767635734"/>
+          <c:h val="0.77235976763573411"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2591,11 +2591,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93093888"/>
-        <c:axId val="93095808"/>
+        <c:axId val="66351104"/>
+        <c:axId val="66353024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93093888"/>
+        <c:axId val="66351104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,12 +2628,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93095808"/>
+        <c:crossAx val="66353024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93095808"/>
+        <c:axId val="66353024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2676,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93093888"/>
+        <c:crossAx val="66351104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2698,10 +2698,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89408588248331888"/>
-          <c:y val="0.3983750380436944"/>
+          <c:x val="0.89408588248331899"/>
+          <c:y val="0.39837503804369445"/>
           <c:w val="9.4910655217460005E-2"/>
-          <c:h val="0.13821174789271043"/>
+          <c:h val="0.13821174789271046"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2766,7 +2766,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3166,7 +3166,7 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3424,18 +3424,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="10"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="69" t="s">
+      <c r="J5" s="69"/>
+      <c r="K5" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69" t="s">
+      <c r="L5" s="73"/>
+      <c r="M5" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="70"/>
+      <c r="N5" s="77"/>
     </row>
     <row r="6" spans="3:14" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -3453,20 +3453,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="79">
+      <c r="I6" s="70">
         <v>3000</v>
       </c>
-      <c r="J6" s="79"/>
-      <c r="K6" s="71">
+      <c r="J6" s="70"/>
+      <c r="K6" s="74">
         <f>I6*E10+E9</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71">
+      <c r="L6" s="74"/>
+      <c r="M6" s="74">
         <f>I6/10</f>
         <v>300</v>
       </c>
-      <c r="N6" s="72"/>
+      <c r="N6" s="78"/>
     </row>
     <row r="7" spans="3:14" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -3489,20 +3489,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="71">
         <v>3000</v>
       </c>
-      <c r="J7" s="80"/>
-      <c r="K7" s="73">
+      <c r="J7" s="71"/>
+      <c r="K7" s="75">
         <f>I7*E13+E12</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73">
+      <c r="L7" s="75"/>
+      <c r="M7" s="75">
         <f>I7/10</f>
         <v>300</v>
       </c>
-      <c r="N7" s="74"/>
+      <c r="N7" s="79"/>
     </row>
     <row r="8" spans="3:14">
       <c r="C8" s="42" t="s">
@@ -3517,18 +3517,18 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="81" t="s">
+      <c r="I8" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="81"/>
-      <c r="K8" s="75" t="s">
+      <c r="J8" s="72"/>
+      <c r="K8" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75" t="s">
+      <c r="L8" s="76"/>
+      <c r="M8" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="76"/>
+      <c r="N8" s="80"/>
     </row>
     <row r="9" spans="3:14" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -3545,20 +3545,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="80">
+      <c r="I9" s="71">
         <v>20</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="73">
+      <c r="J9" s="71"/>
+      <c r="K9" s="75">
         <f>I9/(E14+E15)*E15*1000/D6+E16</f>
         <v>339.23926380368101</v>
       </c>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73">
+      <c r="L9" s="75"/>
+      <c r="M9" s="75">
         <f>I9/10</f>
         <v>2</v>
       </c>
-      <c r="N9" s="77"/>
+      <c r="N9" s="81"/>
     </row>
     <row r="10" spans="3:14">
       <c r="C10" s="43" t="s">
@@ -3792,21 +3792,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add 5LEDs Full, in suspend mode, DSG mos still turn on.
</commit_message>
<xml_diff>
--- a/New_LEVD1_measement.xlsx
+++ b/New_LEVD1_measement.xlsx
@@ -7,20 +7,21 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="19395" windowHeight="8055"/>
   </bookViews>
   <sheets>
-    <sheet name="校正用" sheetId="7" r:id="rId1"/>
-    <sheet name="LEVD1_36V薄_FW設定值" sheetId="6" r:id="rId2"/>
-    <sheet name=" NTC Thermistor" sheetId="3" r:id="rId3"/>
-    <sheet name="實測電流" sheetId="4" r:id="rId4"/>
-    <sheet name="CHG DSG OP" sheetId="1" r:id="rId5"/>
-    <sheet name="Voltage" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId7"/>
+    <sheet name="Current校正用" sheetId="8" r:id="rId1"/>
+    <sheet name="Voltage校正用" sheetId="7" r:id="rId2"/>
+    <sheet name="LEVD1_36V薄_FW設定值" sheetId="6" r:id="rId3"/>
+    <sheet name=" NTC Thermistor" sheetId="3" r:id="rId4"/>
+    <sheet name="實測電流" sheetId="4" r:id="rId5"/>
+    <sheet name="CHG DSG OP" sheetId="1" r:id="rId6"/>
+    <sheet name="Voltage" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="160">
   <si>
     <t>R-sense</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -556,10 +557,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ADC 理論讀值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>輸入ADC讀值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -573,6 +570,62 @@
   </si>
   <si>
     <t>理論值=實際值-Offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add, length, flash sec.,offset, value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e0 03 01 18 fb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mA to ADC ==&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain: 68</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain: 120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理論電流(mA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>輸入實際電流(mA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e0 03 01 16 fb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e0 03 01 17 fb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC 理論值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -583,7 +636,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -621,6 +674,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF1D1884"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -1079,7 +1140,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1272,6 +1333,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1326,6 +1393,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1354,7 +1424,7 @@
           <c:x val="7.2207084468664848E-2"/>
           <c:y val="6.5645584362161905E-2"/>
           <c:w val="0.60354223433242504"/>
-          <c:h val="0.81619343223621377"/>
+          <c:h val="0.81619343223621399"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1629,11 +1699,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64291200"/>
-        <c:axId val="64293120"/>
+        <c:axId val="81260928"/>
+        <c:axId val="81262848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64291200"/>
+        <c:axId val="81260928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,12 +1736,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64293120"/>
+        <c:crossAx val="81262848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64293120"/>
+        <c:axId val="81262848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1784,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64291200"/>
+        <c:crossAx val="81260928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1736,7 +1806,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72070844686648605"/>
+          <c:x val="0.72070844686648639"/>
           <c:y val="0.41794355377243081"/>
           <c:w val="0.26839237057220738"/>
           <c:h val="0.11159749341567524"/>
@@ -1804,7 +1874,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,8 +1892,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10252109253634827"/>
           <c:y val="7.6923269539436984E-2"/>
-          <c:w val="0.5008407471447841"/>
-          <c:h val="0.78461734930225546"/>
+          <c:w val="0.50084074714478433"/>
+          <c:h val="0.78461734930225513"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2170,11 +2240,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64337792"/>
-        <c:axId val="65929216"/>
+        <c:axId val="83019648"/>
+        <c:axId val="83030016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64337792"/>
+        <c:axId val="83019648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,12 +2277,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65929216"/>
+        <c:crossAx val="83030016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65929216"/>
+        <c:axId val="83030016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2325,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64337792"/>
+        <c:crossAx val="83019648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2277,9 +2347,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65210137547710134"/>
+          <c:x val="0.65210137547710156"/>
           <c:y val="0.40512921957436798"/>
-          <c:w val="0.33445405597923528"/>
+          <c:w val="0.3344540559792355"/>
           <c:h val="0.13076955821704281"/>
         </c:manualLayout>
       </c:layout>
@@ -2345,7 +2415,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2361,10 +2431,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2902387340947603E-2"/>
-          <c:y val="8.1301028172182599E-2"/>
+          <c:x val="7.2902387340947644E-2"/>
+          <c:y val="8.1301028172182641E-2"/>
           <c:w val="0.79229764355444865"/>
-          <c:h val="0.77235976763573411"/>
+          <c:h val="0.77235976763573433"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2591,11 +2661,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="66351104"/>
-        <c:axId val="66353024"/>
+        <c:axId val="85356544"/>
+        <c:axId val="85358464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66351104"/>
+        <c:axId val="85356544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,12 +2698,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66353024"/>
+        <c:crossAx val="85358464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66353024"/>
+        <c:axId val="85358464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2746,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66351104"/>
+        <c:crossAx val="85356544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2698,10 +2768,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89408588248331899"/>
-          <c:y val="0.39837503804369445"/>
+          <c:x val="0.89408588248331922"/>
+          <c:y val="0.39837503804369456"/>
           <c:w val="9.4910655217460005E-2"/>
-          <c:h val="0.13821174789271046"/>
+          <c:h val="0.13821174789271051"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2766,7 +2836,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3166,7 +3236,184 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10">
+      <c r="C2" s="60"/>
+    </row>
+    <row r="3" spans="3:10">
+      <c r="C3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="61">
+        <v>0.16383900000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="61">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="84">
+        <f>E3</f>
+        <v>0.16383900000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="17.25" thickBot="1"/>
+    <row r="8" spans="3:10" ht="17.25" thickTop="1">
+      <c r="C8" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="67"/>
+      <c r="E8" s="63">
+        <v>3000</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="70"/>
+      <c r="J8" s="62">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="69"/>
+      <c r="E9" s="64">
+        <f>ROUND(E8*E6,0)</f>
+        <v>492</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="70"/>
+      <c r="J9">
+        <f>ROUND(J8/E6,0)</f>
+        <v>4968</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="C10" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="69"/>
+      <c r="E10" s="65">
+        <v>494</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="C11" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="69"/>
+      <c r="E11" s="64">
+        <f>E10-E9</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" t="str">
+        <f>DEC2HEX(E11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="17.25" thickBot="1">
+      <c r="C12" s="45"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+    </row>
+    <row r="13" spans="3:10" ht="17.25" thickTop="1"/>
+    <row r="15" spans="3:10">
+      <c r="H15" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="I16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9">
+      <c r="H17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3198,77 +3445,77 @@
     </row>
     <row r="5" spans="3:10" ht="17.25" thickBot="1"/>
     <row r="6" spans="3:10" ht="17.25" thickTop="1">
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="63">
         <v>36000</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="68"/>
+      <c r="I6" s="70"/>
       <c r="J6" s="62">
         <v>814</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="66" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="67"/>
+      <c r="C7" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="69"/>
       <c r="E7" s="58">
         <f>ROUND(E6*E4,0)</f>
         <v>611</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="68"/>
+      <c r="I7" s="70"/>
       <c r="J7">
         <f>ROUND(J6/E4,0)</f>
         <v>47990</v>
       </c>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="D8" s="67"/>
+      <c r="C8" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="69"/>
       <c r="E8" s="59">
-        <v>597</v>
+        <v>615</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="67"/>
+      <c r="C9" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="69"/>
       <c r="E9" s="58">
         <f>E8-E7</f>
-        <v>-14</v>
+        <v>4</v>
       </c>
       <c r="F9" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" t="str">
         <f>DEC2HEX(E9)</f>
-        <v>FFFFFFFFF2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="17.25" thickBot="1">
       <c r="C10" s="45"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
@@ -3284,6 +3531,9 @@
       <c r="F13" t="s">
         <v>55</v>
       </c>
+      <c r="I13" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="14" spans="3:10">
       <c r="C14">
@@ -3295,6 +3545,9 @@
       <c r="F14">
         <f>D14/(C14*1000)</f>
         <v>1.7125000000000001E-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="3:10">
@@ -3348,7 +3601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:N50"/>
   <sheetViews>
@@ -3424,18 +3677,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="10"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="69"/>
-      <c r="K5" s="73" t="s">
+      <c r="J5" s="71"/>
+      <c r="K5" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73" t="s">
+      <c r="L5" s="75"/>
+      <c r="M5" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="77"/>
+      <c r="N5" s="79"/>
     </row>
     <row r="6" spans="3:14" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -3453,20 +3706,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="70">
+      <c r="I6" s="72">
         <v>3000</v>
       </c>
-      <c r="J6" s="70"/>
-      <c r="K6" s="74">
+      <c r="J6" s="72"/>
+      <c r="K6" s="76">
         <f>I6*E10+E9</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74">
+      <c r="L6" s="76"/>
+      <c r="M6" s="76">
         <f>I6/10</f>
         <v>300</v>
       </c>
-      <c r="N6" s="78"/>
+      <c r="N6" s="80"/>
     </row>
     <row r="7" spans="3:14" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -3489,20 +3742,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="73">
         <v>3000</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="75">
+      <c r="J7" s="73"/>
+      <c r="K7" s="77">
         <f>I7*E13+E12</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75">
+      <c r="L7" s="77"/>
+      <c r="M7" s="77">
         <f>I7/10</f>
         <v>300</v>
       </c>
-      <c r="N7" s="79"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="3:14">
       <c r="C8" s="42" t="s">
@@ -3517,18 +3770,18 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="72" t="s">
+      <c r="I8" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="76" t="s">
+      <c r="J8" s="74"/>
+      <c r="K8" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76" t="s">
+      <c r="L8" s="78"/>
+      <c r="M8" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="80"/>
+      <c r="N8" s="82"/>
     </row>
     <row r="9" spans="3:14" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -3545,20 +3798,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="71">
+      <c r="I9" s="73">
         <v>20</v>
       </c>
-      <c r="J9" s="71"/>
-      <c r="K9" s="75">
+      <c r="J9" s="73"/>
+      <c r="K9" s="77">
         <f>I9/(E14+E15)*E15*1000/D6+E16</f>
         <v>339.23926380368101</v>
       </c>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75">
+      <c r="L9" s="77"/>
+      <c r="M9" s="77">
         <f>I9/10</f>
         <v>2</v>
       </c>
-      <c r="N9" s="81"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="3:14">
       <c r="C10" s="43" t="s">
@@ -3814,7 +4067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -4325,7 +4578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H72"/>
   <sheetViews>
@@ -5461,7 +5714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:AB53"/>
   <sheetViews>
@@ -7590,7 +7843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J82"/>
   <sheetViews>
@@ -9927,7 +10180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:M43"/>
   <sheetViews>

</xml_diff>

<commit_message>
2nd level samples final Version 36V -> 4LED, 4LED(5LED include red LED), 5LED separate.
</commit_message>
<xml_diff>
--- a/New_LEVD1_measement.xlsx
+++ b/New_LEVD1_measement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="161">
   <si>
     <t>R-sense</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -577,10 +577,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>e0 03 01 18 fb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Current</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -613,19 +609,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>e0 03 01 16 fb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CHG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>e0 03 01 17 fb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ADC 理論值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">e0 03 01 18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>fb</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">e0 03 01 16 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>fb</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">e0 03 01 17 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>fb</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C Address : 0x48</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -636,7 +676,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -682,6 +722,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -1339,16 +1386,19 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1393,9 +1443,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1424,7 +1471,7 @@
           <c:x val="7.2207084468664848E-2"/>
           <c:y val="6.5645584362161905E-2"/>
           <c:w val="0.60354223433242504"/>
-          <c:h val="0.81619343223621399"/>
+          <c:h val="0.81619343223621421"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1699,11 +1746,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81260928"/>
-        <c:axId val="81262848"/>
+        <c:axId val="74040064"/>
+        <c:axId val="74041984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81260928"/>
+        <c:axId val="74040064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,12 +1783,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81262848"/>
+        <c:crossAx val="74041984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81262848"/>
+        <c:axId val="74041984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1831,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81260928"/>
+        <c:crossAx val="74040064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1806,7 +1853,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72070844686648639"/>
+          <c:x val="0.72070844686648672"/>
           <c:y val="0.41794355377243081"/>
           <c:w val="0.26839237057220738"/>
           <c:h val="0.11159749341567524"/>
@@ -1874,7 +1921,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1892,8 +1939,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10252109253634827"/>
           <c:y val="7.6923269539436984E-2"/>
-          <c:w val="0.50084074714478433"/>
-          <c:h val="0.78461734930225513"/>
+          <c:w val="0.50084074714478455"/>
+          <c:h val="0.78461734930225469"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2240,11 +2287,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83019648"/>
-        <c:axId val="83030016"/>
+        <c:axId val="74205440"/>
+        <c:axId val="74224000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83019648"/>
+        <c:axId val="74205440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,12 +2324,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83030016"/>
+        <c:crossAx val="74224000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83030016"/>
+        <c:axId val="74224000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2325,7 +2372,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83019648"/>
+        <c:crossAx val="74205440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2347,9 +2394,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65210137547710156"/>
+          <c:x val="0.6521013754771019"/>
           <c:y val="0.40512921957436798"/>
-          <c:w val="0.3344540559792355"/>
+          <c:w val="0.33445405597923572"/>
           <c:h val="0.13076955821704281"/>
         </c:manualLayout>
       </c:layout>
@@ -2415,7 +2462,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2431,10 +2478,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2902387340947644E-2"/>
-          <c:y val="8.1301028172182641E-2"/>
+          <c:x val="7.29023873409477E-2"/>
+          <c:y val="8.1301028172182682E-2"/>
           <c:w val="0.79229764355444865"/>
-          <c:h val="0.77235976763573433"/>
+          <c:h val="0.77235976763573455"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2661,11 +2708,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85356544"/>
-        <c:axId val="85358464"/>
+        <c:axId val="75747712"/>
+        <c:axId val="75749632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85356544"/>
+        <c:axId val="75747712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,12 +2745,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85358464"/>
+        <c:crossAx val="75749632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85358464"/>
+        <c:axId val="75749632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2746,7 +2793,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85356544"/>
+        <c:crossAx val="75747712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2768,10 +2815,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89408588248331922"/>
-          <c:y val="0.39837503804369456"/>
+          <c:x val="0.89408588248331944"/>
+          <c:y val="0.39837503804369467"/>
           <c:w val="9.4910655217460005E-2"/>
-          <c:h val="0.13821174789271051"/>
+          <c:h val="0.13821174789271057"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2836,7 +2883,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3236,7 +3283,7 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3250,7 +3297,7 @@
     </row>
     <row r="3" spans="3:10">
       <c r="C3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
         <v>137</v>
@@ -3259,15 +3306,15 @@
         <v>0.16383900000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="3:10">
       <c r="C4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
         <v>137</v>
@@ -3276,82 +3323,82 @@
         <v>9.2799999999999994E-2</v>
       </c>
       <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" t="s">
         <v>149</v>
-      </c>
-      <c r="H4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" t="s">
         <v>152</v>
       </c>
-      <c r="D6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="84">
+      <c r="E6" s="66">
         <f>E3</f>
         <v>0.16383900000000001</v>
       </c>
     </row>
     <row r="7" spans="3:10" ht="17.25" thickBot="1"/>
     <row r="8" spans="3:10" ht="17.25" thickTop="1">
-      <c r="C8" s="66" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="67"/>
+      <c r="C8" s="69" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="70"/>
       <c r="E8" s="63">
         <v>3000</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="62">
         <v>814</v>
       </c>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="69"/>
+      <c r="C9" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="68"/>
       <c r="E9" s="64">
         <f>ROUND(E8*E6,0)</f>
         <v>492</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="70" t="s">
-        <v>154</v>
-      </c>
-      <c r="I9" s="70"/>
+      <c r="H9" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="I9" s="71"/>
       <c r="J9">
         <f>ROUND(J8/E6,0)</f>
         <v>4968</v>
       </c>
     </row>
     <row r="10" spans="3:10">
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="69"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="65">
-        <v>494</v>
+        <v>270</v>
       </c>
       <c r="F10" s="64"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="64">
         <f>E10-E9</f>
-        <v>2</v>
+        <v>-222</v>
       </c>
       <c r="F11" s="64" t="s">
         <v>144</v>
@@ -3359,7 +3406,7 @@
       <c r="G11" s="15"/>
       <c r="H11" t="str">
         <f>DEC2HEX(E11)</f>
-        <v>2</v>
+        <v>FFFFFFFF22</v>
       </c>
     </row>
     <row r="12" spans="3:10" ht="17.25" thickBot="1">
@@ -3374,10 +3421,10 @@
     <row r="13" spans="3:10" ht="17.25" thickTop="1"/>
     <row r="15" spans="3:10">
       <c r="H15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="3:10">
@@ -3390,17 +3437,17 @@
         <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3413,7 +3460,7 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:D8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3445,62 +3492,62 @@
     </row>
     <row r="5" spans="3:10" ht="17.25" thickBot="1"/>
     <row r="6" spans="3:10" ht="17.25" thickTop="1">
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="67"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="63">
         <v>36000</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="70"/>
+      <c r="I6" s="71"/>
       <c r="J6" s="62">
         <v>814</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="69"/>
+      <c r="C7" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="68"/>
       <c r="E7" s="58">
         <f>ROUND(E6*E4,0)</f>
         <v>611</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7">
         <f>ROUND(J6/E4,0)</f>
         <v>47990</v>
       </c>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="59">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="69"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="58">
         <f>E8-E7</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F9" s="58" t="s">
         <v>144</v>
@@ -3508,7 +3555,7 @@
       <c r="G9" s="15"/>
       <c r="H9" t="str">
         <f>DEC2HEX(E9)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="17.25" thickBot="1">
@@ -3520,7 +3567,11 @@
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="3:10" ht="17.25" thickTop="1"/>
+    <row r="11" spans="3:10" ht="17.25" thickTop="1">
+      <c r="I11" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="13" spans="3:10">
       <c r="C13" t="s">
         <v>136</v>
@@ -3532,7 +3583,7 @@
         <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="3:10">
@@ -3677,18 +3728,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="10"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="71"/>
-      <c r="K5" s="75" t="s">
+      <c r="J5" s="72"/>
+      <c r="K5" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75" t="s">
+      <c r="L5" s="76"/>
+      <c r="M5" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="79"/>
+      <c r="N5" s="80"/>
     </row>
     <row r="6" spans="3:14" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -3706,20 +3757,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="73">
         <v>3000</v>
       </c>
-      <c r="J6" s="72"/>
-      <c r="K6" s="76">
+      <c r="J6" s="73"/>
+      <c r="K6" s="77">
         <f>I6*E10+E9</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76">
+      <c r="L6" s="77"/>
+      <c r="M6" s="77">
         <f>I6/10</f>
         <v>300</v>
       </c>
-      <c r="N6" s="80"/>
+      <c r="N6" s="81"/>
     </row>
     <row r="7" spans="3:14" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -3742,20 +3793,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="74">
         <v>3000</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="77">
+      <c r="J7" s="74"/>
+      <c r="K7" s="78">
         <f>I7*E13+E12</f>
         <v>278.52800000000002</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77">
+      <c r="L7" s="78"/>
+      <c r="M7" s="78">
         <f>I7/10</f>
         <v>300</v>
       </c>
-      <c r="N7" s="81"/>
+      <c r="N7" s="82"/>
     </row>
     <row r="8" spans="3:14">
       <c r="C8" s="42" t="s">
@@ -3770,18 +3821,18 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="74" t="s">
+      <c r="I8" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="78" t="s">
+      <c r="J8" s="75"/>
+      <c r="K8" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78" t="s">
+      <c r="L8" s="79"/>
+      <c r="M8" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="82"/>
+      <c r="N8" s="83"/>
     </row>
     <row r="9" spans="3:14" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -3798,20 +3849,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="73">
+      <c r="I9" s="74">
         <v>20</v>
       </c>
-      <c r="J9" s="73"/>
-      <c r="K9" s="77">
+      <c r="J9" s="74"/>
+      <c r="K9" s="78">
         <f>I9/(E14+E15)*E15*1000/D6+E16</f>
         <v>339.23926380368101</v>
       </c>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77">
+      <c r="L9" s="78"/>
+      <c r="M9" s="78">
         <f>I9/10</f>
         <v>2</v>
       </c>
-      <c r="N9" s="83"/>
+      <c r="N9" s="84"/>
     </row>
     <row r="10" spans="3:14">
       <c r="C10" s="43" t="s">

</xml_diff>